<commit_message>
Se cambio prediccion minima a 0.5
</commit_message>
<xml_diff>
--- a/prediccion_Algoritmos.xlsx
+++ b/prediccion_Algoritmos.xlsx
@@ -732,8 +732,8 @@
       <c r="F14" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="3">
-        <v>0.552</v>
+      <c r="G14" s="2">
+        <v>0.548</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -779,7 +779,7 @@
         <v>7</v>
       </c>
       <c r="G16" s="2">
-        <v>0.896</v>
+        <v>0.928</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -940,7 +940,7 @@
         <v>7</v>
       </c>
       <c r="G23" s="2">
-        <v>0.856</v>
+        <v>0.888</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1008,8 +1008,8 @@
       <c r="F26" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="3">
-        <v>0.552</v>
+      <c r="G26" s="2">
+        <v>0.548</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1032,7 +1032,7 @@
         <v>7</v>
       </c>
       <c r="G27" s="2">
-        <v>0.716</v>
+        <v>0.708</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1193,7 +1193,7 @@
         <v>7</v>
       </c>
       <c r="G34" s="2">
-        <v>0.716</v>
+        <v>0.708</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1376,8 +1376,8 @@
       <c r="F42" t="s">
         <v>7</v>
       </c>
-      <c r="G42" s="3">
-        <v>0.552</v>
+      <c r="G42" s="2">
+        <v>0.548</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1422,8 +1422,8 @@
       <c r="F44" t="s">
         <v>7</v>
       </c>
-      <c r="G44" s="3">
-        <v>0.552</v>
+      <c r="G44" s="2">
+        <v>0.548</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1492,7 +1492,7 @@
         <v>7</v>
       </c>
       <c r="G47" s="2">
-        <v>0.928</v>
+        <v>0.972</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1597,7 +1597,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generated normal distribution for grades
</commit_message>
<xml_diff>
--- a/prediccion_Algoritmos.xlsx
+++ b/prediccion_Algoritmos.xlsx
@@ -733,7 +733,7 @@
         <v>7</v>
       </c>
       <c r="G14" s="2">
-        <v>0.548</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -779,7 +779,7 @@
         <v>7</v>
       </c>
       <c r="G16" s="2">
-        <v>0.928</v>
+        <v>0.864</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -940,7 +940,7 @@
         <v>7</v>
       </c>
       <c r="G23" s="2">
-        <v>0.888</v>
+        <v>0.8120000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1009,7 +1009,7 @@
         <v>7</v>
       </c>
       <c r="G26" s="2">
-        <v>0.548</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1032,7 +1032,7 @@
         <v>7</v>
       </c>
       <c r="G27" s="2">
-        <v>0.708</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1193,7 +1193,7 @@
         <v>7</v>
       </c>
       <c r="G34" s="2">
-        <v>0.708</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1377,7 +1377,7 @@
         <v>7</v>
       </c>
       <c r="G42" s="2">
-        <v>0.548</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1423,7 +1423,7 @@
         <v>7</v>
       </c>
       <c r="G44" s="2">
-        <v>0.548</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1492,7 +1492,7 @@
         <v>7</v>
       </c>
       <c r="G47" s="2">
-        <v>0.972</v>
+        <v>0.9320000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:7">

</xml_diff>